<commit_message>
updated lab and added 100 and 500 to report
</commit_message>
<xml_diff>
--- a/CollaborativeFilteringAndRecommenderSystem/labreport.xlsx
+++ b/CollaborativeFilteringAndRecommenderSystem/labreport.xlsx
@@ -73,28 +73,21 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.8333333333333329E-2"/>
-          <c:y val="5.6030183727034118E-2"/>
-          <c:w val="0.76123053368328963"/>
-          <c:h val="0.89719889180519097"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Actual</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
@@ -162,7 +155,19 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Predicted</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:yVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$21</c:f>
@@ -233,74 +238,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>SERIES2</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-          </c:trendline>
-          <c:trendline>
-            <c:trendlineType val="linear"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$1:$D$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$1:$C$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="71475200"/>
-        <c:axId val="71473408"/>
+        <c:axId val="63376000"/>
+        <c:axId val="63377792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71475200"/>
+        <c:axId val="63376000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71473408"/>
+        <c:crossAx val="63377792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71473408"/>
+        <c:axId val="63377792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,16 +261,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71475200"/>
+        <c:crossAx val="63376000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -344,7 +301,7 @@
           </c:spPr>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>Sheet1!$A$25:$A$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -425,90 +382,90 @@
           </c:spPr>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:f>Sheet1!$B$25:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.24659304000000001</c:v>
+                  <c:v>0.36966450000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20801717</c:v>
+                  <c:v>0.32793927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.73152609999999996</c:v>
+                  <c:v>-0.72081523999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.1121736000000002</c:v>
+                  <c:v>-2.2089026</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5941455</c:v>
+                  <c:v>1.690623</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.7625966</c:v>
+                  <c:v>-0.84581620000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5000167</c:v>
+                  <c:v>1.5783780999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.4591253000000002</c:v>
+                  <c:v>1.4338918</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8374401</c:v>
+                  <c:v>1.9107057000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.57805479999999998</c:v>
+                  <c:v>-0.36762013999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3003591999999999</c:v>
+                  <c:v>1.3802220999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6731178</c:v>
+                  <c:v>1.7740005000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.1109684</c:v>
+                  <c:v>2.0507955999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.5185435</c:v>
+                  <c:v>1.0045854999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.93403670000000005</c:v>
+                  <c:v>-0.56155175000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.3124449999999999</c:v>
+                  <c:v>3.4265869000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1988020000000001</c:v>
+                  <c:v>2.0462554000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0675593999999999</c:v>
+                  <c:v>1.0194220000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.4036054</c:v>
+                  <c:v>0.38465807000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.7151035</c:v>
+                  <c:v>0.81699869999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="76632832"/>
-        <c:axId val="76622848"/>
+        <c:axId val="63398272"/>
+        <c:axId val="63399808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="76632832"/>
+        <c:axId val="63398272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76622848"/>
+        <c:crossAx val="63399808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="76622848"/>
+        <c:axId val="63399808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,7 +473,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76632832"/>
+        <c:crossAx val="63398272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -529,7 +486,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -556,218 +513,6 @@
           </c:spPr>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$25:$A$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>8.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.4300000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.86</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-8.83</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.08</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-6.26</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.24</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.08</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.35</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-7.72</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.8099999999999996</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.68</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-3.98</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-0.83</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Predicted</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$25:$B$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>0.36966450000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.32793927</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.72081523999999997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-2.2089026</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.690623</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.84581620000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.5783780999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.4338918</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.9107057000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.36762013999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3802220999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.7740005000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.0507955999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0045854999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.56155175000000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.4265869000000002</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.0462554000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.0194220000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.38465807000000002</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.81699869999999997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-        </c:ser>
-        <c:axId val="81536512"/>
-        <c:axId val="80903552"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="81536512"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80903552"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="80903552"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81536512"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Actual</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:yVal>
-            <c:numRef>
               <c:f>Sheet1!$A$49:$A$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -917,22 +662,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82416384"/>
-        <c:axId val="82267136"/>
+        <c:axId val="63432576"/>
+        <c:axId val="63434112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82416384"/>
+        <c:axId val="63432576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82267136"/>
+        <c:crossAx val="63434112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82267136"/>
+        <c:axId val="63434112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +685,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82416384"/>
+        <c:crossAx val="63432576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -953,13 +698,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1162,31 +907,35 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83195392"/>
-        <c:axId val="83193856"/>
+        <c:axId val="63472000"/>
+        <c:axId val="63473536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83195392"/>
+        <c:axId val="63472000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83193856"/>
+        <c:crossAx val="63473536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83193856"/>
+        <c:axId val="63473536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83195392"/>
+        <c:crossAx val="63472000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1195,13 +944,13 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1404,31 +1153,281 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91234688"/>
-        <c:axId val="82922112"/>
+        <c:axId val="63502592"/>
+        <c:axId val="64159744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91234688"/>
+        <c:axId val="63502592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82922112"/>
+        <c:crossAx val="64159744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82922112"/>
+        <c:axId val="64159744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91234688"/>
+        <c:crossAx val="63502592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.86</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-8.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-6.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.35</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-3.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.83</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.24659304000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20801717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.73152609999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.1121736000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5941455</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.7625966</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5000167</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4591253000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8374401</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.57805479999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.3003591999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6731178</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1109684</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5185435</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.93403670000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3124449999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1988020000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0675593999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.4036054</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.7151035</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>line</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="118529024"/>
+        <c:axId val="90060288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="118529024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90060288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="90060288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+          <c:min val="-10"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="118529024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1445,36 +1444,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -1499,7 +1468,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1529,7 +1498,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1559,7 +1528,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1589,7 +1558,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1611,6 +1580,36 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1916,7 +1915,7 @@
   <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>